<commit_message>
updated isochrones and free health map
</commit_message>
<xml_diff>
--- a/shinyapp/data/resourcecost.xlsx
+++ b/shinyapp/data/resourcecost.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amandaljuba/Downloads/DSPG-R-Training/2022_DSPG_Loudoun/shinyapp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BDD7AE-D873-8D42-83B1-F42A8DFE8ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE72AAB6-E829-3648-80DE-00D7FAB5C254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25920" windowHeight="15880" xr2:uid="{BAAF709D-C9C5-8D48-B85E-C6C35467C9B5}"/>
+    <workbookView xWindow="820" yWindow="500" windowWidth="14340" windowHeight="16280" firstSheet="1" activeTab="3" xr2:uid="{BAAF709D-C9C5-8D48-B85E-C6C35467C9B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Health Free" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="383">
   <si>
     <t>Food Pantry</t>
   </si>
@@ -817,9 +817,6 @@
     <t>24419 Millstream Drive, Aldie, VA 20105</t>
   </si>
   <si>
-    <t>Grief Support</t>
-  </si>
-  <si>
     <t>Individual or Family grief counseling</t>
   </si>
   <si>
@@ -835,24 +832,15 @@
     <t>795 Center Street, Herndon, VA 20170</t>
   </si>
   <si>
-    <t>Domestic Violence Program</t>
-  </si>
-  <si>
     <t>Crisis Counseling, Safety planning, Legal representation, Court advocacy, Translation services, Financial assistance</t>
   </si>
   <si>
-    <t xml:space="preserve">Supportive Tools for Advancement and Restoration </t>
-  </si>
-  <si>
     <t>By Your Side Ministries seeks to aid in the development of life skills in single, young adult mothers (ages 16 -30) in under-served communities via mentoring, workshops and seminars in the areas of education &amp; career planning, money management, social skills development and wellness.</t>
   </si>
   <si>
     <t>26 Fairfax Street Southeast, Leesburg, VA 20175</t>
   </si>
   <si>
-    <t>Offender Services</t>
-  </si>
-  <si>
     <t>Employment assistance, help obtainign uniforms, Emrgency assistance, Counseling to help deal with emotional and cognitive effects of incarceration</t>
   </si>
   <si>
@@ -865,18 +853,9 @@
     <t>5250 Cherokee Avenue, Lincolnia, VA 22312</t>
   </si>
   <si>
-    <t>Adoption and Mental Health Services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Free 24/7 Counseling for Expectant parents, Mental health counseling for children, Parents and Families, Foster care adoption and domestic Infant adoption </t>
-  </si>
-  <si>
     <t>24/7</t>
   </si>
   <si>
-    <t>44180 Riverside Pkwy, Leesburg, VA 20176</t>
-  </si>
-  <si>
     <t>Supporting Successful Reentry</t>
   </si>
   <si>
@@ -1082,6 +1061,135 @@
   </si>
   <si>
     <t>In the Read-Aloud program, volunteers and kids read great books, selected to support a theme such as onomatopoeia, or superheroes or cats and dogs. Kids and adults share conversations and work on an activity related to the books' theme. And every week, the kids pick a new book for their own.</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>Club</t>
+  </si>
+  <si>
+    <t>Athletics</t>
+  </si>
+  <si>
+    <t>After School Program</t>
+  </si>
+  <si>
+    <t>Latitude4</t>
+  </si>
+  <si>
+    <t>Longitude4</t>
+  </si>
+  <si>
+    <t>Name4</t>
+  </si>
+  <si>
+    <t>Description4</t>
+  </si>
+  <si>
+    <t>Hours4</t>
+  </si>
+  <si>
+    <t>Website4</t>
+  </si>
+  <si>
+    <t>https://www.applefcu.org/</t>
+  </si>
+  <si>
+    <t>https://www.loudounsoccer.com/</t>
+  </si>
+  <si>
+    <t>https://www.sterlingsoccerclub.org/</t>
+  </si>
+  <si>
+    <t>https://www.inova.org/inova-community/community-partnerships/childhood-obesity-prevention</t>
+  </si>
+  <si>
+    <t>https://inmedusa.org/</t>
+  </si>
+  <si>
+    <t>https://loudoun.ext.vt.edu/</t>
+  </si>
+  <si>
+    <t>https://www.ymcadc.org/locations/ymca-fairfax-county-reston/</t>
+  </si>
+  <si>
+    <t>https://library.loudoun.gov/Sterling</t>
+  </si>
+  <si>
+    <t>https://www.findhelp.org/northern-virginia-family-service-%2528nvfs%2529--sterling-va--read-aloud-program/6027539993067520?postal=20166</t>
+  </si>
+  <si>
+    <t>Resource5</t>
+  </si>
+  <si>
+    <t>Cost5</t>
+  </si>
+  <si>
+    <t>Latitude5</t>
+  </si>
+  <si>
+    <t>Longitude5</t>
+  </si>
+  <si>
+    <t>Name5</t>
+  </si>
+  <si>
+    <t>Description5</t>
+  </si>
+  <si>
+    <t>Hours5</t>
+  </si>
+  <si>
+    <t>Address5</t>
+  </si>
+  <si>
+    <t>Website5</t>
+  </si>
+  <si>
+    <t>https://yourfamilymed.com/contact/lansdowne/</t>
+  </si>
+  <si>
+    <t>Capital Caring Adler Center</t>
+  </si>
+  <si>
+    <t>https://www.dewberry.com/projects/capital-caring-health-adler-center-for-caring-on-the-van-metre-campus</t>
+  </si>
+  <si>
+    <t>FAITH</t>
+  </si>
+  <si>
+    <t>https://www.faithus.org/programs/domestic-violence-program/</t>
+  </si>
+  <si>
+    <t>By Your Side Ministries</t>
+  </si>
+  <si>
+    <t>https://www.findhelp.org/by-your-side-ministries-inc--sterling-va--supportive-tools-for-advancement-and-restoration-%2528star%2529/5123958760275968?postal=20163</t>
+  </si>
+  <si>
+    <t>Connections Health Center</t>
+  </si>
+  <si>
+    <t>http://www.connectionshealthcenter.com/mental-health-services-our-services</t>
+  </si>
+  <si>
+    <t>Adoptions Together</t>
+  </si>
+  <si>
+    <t>https://www.adoptionstogether.org/</t>
+  </si>
+  <si>
+    <t>Those who are formerly incarcerated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Counseling for expectant parents, Mental health counseling for children, parents and Families, foster care adoption and domestic infant adoption </t>
+  </si>
+  <si>
+    <t>Address4</t>
   </si>
 </sst>
 </file>
@@ -1195,7 +1303,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1218,6 +1326,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1535,7 +1644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D4202D-4282-9E4F-97ED-41B512CE5383}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -3355,261 +3464,292 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49DF9615-B217-A24B-BE00-FA59CC559B4F}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>154</v>
       </c>
       <c r="B1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C1" t="s">
         <v>159</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>151</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>152</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>153</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>155</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>39.023605799999999</v>
+      </c>
+      <c r="F2">
+        <v>-77.400994999999995</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="H2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" t="s">
+        <v>278</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>39.110369400000003</v>
+      </c>
+      <c r="F3">
+        <v>-77.565443999999999</v>
+      </c>
+      <c r="G3" t="s">
+        <v>279</v>
+      </c>
+      <c r="H3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="C4" t="s">
         <v>281</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>39.023605799999999</v>
-      </c>
-      <c r="E2">
-        <v>-77.400994999999995</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>38.865062399999999</v>
+      </c>
+      <c r="F4">
+        <v>-77.358749000000003</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B5" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="C5" t="s">
         <v>284</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>39.0403175</v>
+      </c>
+      <c r="F5">
+        <v>-77.486816000000005</v>
+      </c>
+      <c r="G5" t="s">
         <v>285</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>39.110369400000003</v>
-      </c>
-      <c r="E3">
-        <v>-77.565443999999999</v>
-      </c>
-      <c r="F3" t="s">
+    </row>
+    <row r="6" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="G3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D6" s="11">
+        <v>1</v>
+      </c>
+      <c r="E6" s="11">
+        <v>39.013576499999999</v>
+      </c>
+      <c r="F6" s="11">
+        <v>-77.384056000000001</v>
+      </c>
+      <c r="G6" s="12" t="s">
         <v>288</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>38.865062399999999</v>
-      </c>
-      <c r="E4">
-        <v>-77.358749000000003</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="H6" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="G4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+    </row>
+    <row r="7" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
         <v>290</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>291</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>39.0403175</v>
-      </c>
-      <c r="E5">
-        <v>-77.486816000000005</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="D7" s="11">
+        <v>1</v>
+      </c>
+      <c r="E7" s="11">
+        <v>38.955991699999998</v>
+      </c>
+      <c r="F7" s="11">
+        <v>-77.368133999999998</v>
+      </c>
+      <c r="G7" s="12" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="409.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
+      <c r="H7" s="11" t="s">
         <v>293</v>
       </c>
-      <c r="B6" s="11" t="s">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
         <v>294</v>
       </c>
-      <c r="C6" s="11">
-        <v>1</v>
-      </c>
-      <c r="D6" s="11">
-        <v>39.013576499999999</v>
-      </c>
-      <c r="E6" s="11">
-        <v>-77.384056000000001</v>
-      </c>
-      <c r="F6" s="12" t="s">
+      <c r="B8" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>295</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="D8" s="11">
+        <v>1</v>
+      </c>
+      <c r="E8" s="11">
+        <v>38.9531086</v>
+      </c>
+      <c r="F8" s="11">
+        <v>-77.346993999999995</v>
+      </c>
+      <c r="G8" s="13" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+      <c r="H8" t="s">
         <v>297</v>
       </c>
-      <c r="B7" s="11" t="s">
+    </row>
+    <row r="9" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
         <v>298</v>
       </c>
-      <c r="C7" s="11">
-        <v>1</v>
-      </c>
-      <c r="D7" s="11">
-        <v>38.955991699999998</v>
-      </c>
-      <c r="E7" s="11">
-        <v>-77.368133999999998</v>
-      </c>
-      <c r="F7" s="12" t="s">
+      <c r="B9" s="11" t="s">
+        <v>343</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>299</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="D9" s="11">
+        <v>1</v>
+      </c>
+      <c r="E9" s="11">
+        <v>39.0611465</v>
+      </c>
+      <c r="F9" s="11">
+        <v>-77.552453999999997</v>
+      </c>
+      <c r="G9" s="12" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
+      <c r="H9" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="B8" s="11" t="s">
+    </row>
+    <row r="10" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="C8" s="11">
-        <v>1</v>
-      </c>
-      <c r="D8" s="11">
-        <v>38.9531086</v>
-      </c>
-      <c r="E8" s="11">
-        <v>-77.346993999999995</v>
-      </c>
-      <c r="F8" s="13" t="s">
+      <c r="B10" s="11" t="s">
+        <v>342</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>303</v>
       </c>
-      <c r="G8" t="s">
+      <c r="D10" s="11">
+        <v>1</v>
+      </c>
+      <c r="E10" s="11">
+        <v>38.925209099999996</v>
+      </c>
+      <c r="F10" s="11">
+        <v>-77.520797999999999</v>
+      </c>
+      <c r="G10" s="12" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
+      <c r="H10" s="11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
         <v>305</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B11" s="11" t="s">
+        <v>342</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>306</v>
       </c>
-      <c r="C9" s="11">
-        <v>1</v>
-      </c>
-      <c r="D9" s="11">
-        <v>39.0611465</v>
-      </c>
-      <c r="E9" s="11">
-        <v>-77.552453999999997</v>
-      </c>
-      <c r="F9" s="12" t="s">
+      <c r="D11" s="11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="11">
+        <v>38.847721700000001</v>
+      </c>
+      <c r="F11" s="11">
+        <v>-77.310794000000001</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>307</v>
       </c>
-      <c r="G9" s="11" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
-        <v>309</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>310</v>
-      </c>
-      <c r="C10" s="11">
-        <v>1</v>
-      </c>
-      <c r="D10" s="11">
-        <v>38.925209099999996</v>
-      </c>
-      <c r="E10" s="11">
-        <v>-77.520797999999999</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>311</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
-        <v>312</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>313</v>
-      </c>
-      <c r="C11" s="11">
-        <v>1</v>
-      </c>
-      <c r="D11" s="11">
-        <v>38.847721700000001</v>
-      </c>
-      <c r="E11" s="11">
-        <v>-77.310794000000001</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>314</v>
-      </c>
-      <c r="G11" s="11" t="s">
+      <c r="H11" s="11" t="s">
         <v>126</v>
       </c>
     </row>
@@ -3620,245 +3760,308 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE608C9-15CC-5E48-B239-366E0A11B3B1}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>154</v>
+        <v>347</v>
       </c>
       <c r="B1" t="s">
-        <v>159</v>
+        <v>340</v>
       </c>
       <c r="C1" t="s">
+        <v>382</v>
+      </c>
+      <c r="D1" t="s">
         <v>151</v>
       </c>
-      <c r="D1" t="s">
-        <v>152</v>
-      </c>
       <c r="E1" t="s">
-        <v>153</v>
+        <v>345</v>
       </c>
       <c r="F1" t="s">
-        <v>155</v>
+        <v>346</v>
       </c>
       <c r="G1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>348</v>
+      </c>
+      <c r="H1" t="s">
+        <v>349</v>
+      </c>
+      <c r="I1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" t="s">
+        <v>309</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>39.024802000000001</v>
+      </c>
+      <c r="F2">
+        <v>-77.405699999999996</v>
+      </c>
+      <c r="G2" t="s">
+        <v>310</v>
+      </c>
+      <c r="H2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>311</v>
+      </c>
+      <c r="B3" t="s">
+        <v>343</v>
+      </c>
+      <c r="C3" t="s">
+        <v>312</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>39.092599999999997</v>
+      </c>
+      <c r="F3">
+        <v>-77.553653999999995</v>
+      </c>
+      <c r="G3" t="s">
+        <v>313</v>
+      </c>
+      <c r="H3" t="s">
+        <v>301</v>
+      </c>
+      <c r="I3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>314</v>
+      </c>
+      <c r="B4" t="s">
+        <v>343</v>
+      </c>
+      <c r="C4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>39.015830999999999</v>
+      </c>
+      <c r="F4">
+        <v>-77.375861999999998</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="B2" t="s">
+      <c r="H4" t="s">
         <v>316</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>39.024802000000001</v>
-      </c>
-      <c r="E2">
-        <v>-77.405699999999996</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="I4" s="16" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="G2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B5" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="C5" t="s">
         <v>318</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>39.024825700000001</v>
+      </c>
+      <c r="F5">
+        <v>-77.3927944</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>319</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>39.092599999999997</v>
-      </c>
-      <c r="E3">
-        <v>-77.553653999999995</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="H5" t="s">
         <v>320</v>
       </c>
-      <c r="G3" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="I5" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
         <v>321</v>
       </c>
-      <c r="B4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>39.015830999999999</v>
-      </c>
-      <c r="E4">
-        <v>-77.375861999999998</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="B6" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" t="s">
         <v>322</v>
       </c>
-      <c r="G4" t="s">
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>39.027190400000002</v>
+      </c>
+      <c r="F6">
+        <v>-77.408413999999993</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="H6" t="s">
         <v>324</v>
       </c>
-      <c r="B5" t="s">
+      <c r="I6" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
         <v>325</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>39.024825700000001</v>
-      </c>
-      <c r="E5">
-        <v>-77.3927944</v>
-      </c>
-      <c r="F5" s="14" t="s">
+      <c r="B7" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="C7" t="s">
         <v>326</v>
       </c>
-      <c r="G5" t="s">
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>39.081523900000001</v>
+      </c>
+      <c r="F7">
+        <v>-77.555297999999993</v>
+      </c>
+      <c r="G7" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="H7" t="s">
         <v>328</v>
       </c>
-      <c r="B6" t="s">
+      <c r="I7" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
         <v>329</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>39.027190400000002</v>
-      </c>
-      <c r="E6">
-        <v>-77.408413999999993</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="B8" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>330</v>
       </c>
-      <c r="G6" t="s">
+      <c r="D8" s="11">
+        <v>0</v>
+      </c>
+      <c r="E8" s="11">
+        <v>39.065376299999997</v>
+      </c>
+      <c r="F8" s="11">
+        <v>-77.149856999999997</v>
+      </c>
+      <c r="G8" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="H8" s="11" t="s">
         <v>332</v>
       </c>
-      <c r="B7" t="s">
+      <c r="I8" s="11" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
         <v>333</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>39.081523900000001</v>
-      </c>
-      <c r="E7">
-        <v>-77.555297999999993</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="B9" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="G7" t="s">
+      <c r="D9" s="11">
+        <v>0</v>
+      </c>
+      <c r="E9" s="11">
+        <v>38.9978257</v>
+      </c>
+      <c r="F9" s="11">
+        <v>-77.406756999999999</v>
+      </c>
+      <c r="G9" s="15" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
+      <c r="H9" s="11" t="s">
         <v>336</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="I9" s="11" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="C8" s="11">
-        <v>0</v>
-      </c>
-      <c r="D8" s="11">
-        <v>39.065376299999997</v>
-      </c>
-      <c r="E8" s="11">
-        <v>-77.149856999999997</v>
-      </c>
-      <c r="F8" s="13" t="s">
+      <c r="B10" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>338</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="D10" s="11">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>38.744839399999996</v>
+      </c>
+      <c r="F10">
+        <v>-77.499871799999994</v>
+      </c>
+      <c r="G10" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
-        <v>340</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>341</v>
-      </c>
-      <c r="C9" s="11">
-        <v>0</v>
-      </c>
-      <c r="D9" s="11">
-        <v>38.9978257</v>
-      </c>
-      <c r="E9" s="11">
-        <v>-77.406756999999999</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>342</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>345</v>
-      </c>
-      <c r="C10" s="11">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>38.744839399999996</v>
-      </c>
-      <c r="E10">
-        <v>-77.499871799999994</v>
-      </c>
-      <c r="F10" t="s">
-        <v>346</v>
-      </c>
-      <c r="G10" s="9" t="s">
+      <c r="H10" s="9" t="s">
         <v>126</v>
       </c>
+      <c r="I10" s="11" t="s">
+        <v>359</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I4" r:id="rId1" xr:uid="{BBD7A5D6-79E0-ED47-A9FB-FC9E61025EE0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4254,47 +4457,44 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6631F4BE-4E4B-894D-9D61-34BE7B78F59B}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>150</v>
+        <v>360</v>
       </c>
       <c r="B1" t="s">
-        <v>151</v>
+        <v>361</v>
       </c>
       <c r="C1" t="s">
-        <v>152</v>
+        <v>362</v>
       </c>
       <c r="D1" t="s">
-        <v>153</v>
+        <v>363</v>
       </c>
       <c r="E1" t="s">
-        <v>154</v>
+        <v>364</v>
       </c>
       <c r="F1" t="s">
-        <v>155</v>
+        <v>365</v>
       </c>
       <c r="G1" t="s">
-        <v>156</v>
+        <v>366</v>
       </c>
       <c r="H1" t="s">
-        <v>157</v>
+        <v>367</v>
       </c>
       <c r="I1" t="s">
-        <v>158</v>
-      </c>
-      <c r="J1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>233</v>
       </c>
@@ -4308,10 +4508,10 @@
         <v>-77.547101999999995</v>
       </c>
       <c r="E2" t="s">
+        <v>370</v>
+      </c>
+      <c r="F2" t="s">
         <v>258</v>
-      </c>
-      <c r="F2" t="s">
-        <v>259</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>126</v>
@@ -4319,8 +4519,11 @@
       <c r="H2" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>234</v>
       </c>
@@ -4334,19 +4537,22 @@
         <v>-77.477527100000003</v>
       </c>
       <c r="E3" t="s">
+        <v>260</v>
+      </c>
+      <c r="F3" t="s">
         <v>261</v>
-      </c>
-      <c r="F3" t="s">
-        <v>262</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>126</v>
       </c>
       <c r="H3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>259</v>
+      </c>
+      <c r="I3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>234</v>
       </c>
@@ -4360,19 +4566,22 @@
         <v>-77.385575399999993</v>
       </c>
       <c r="E4" t="s">
-        <v>264</v>
+        <v>372</v>
       </c>
       <c r="F4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>126</v>
       </c>
       <c r="H4" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>262</v>
+      </c>
+      <c r="I4" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>234</v>
       </c>
@@ -4386,10 +4595,10 @@
         <v>-77.347973999999994</v>
       </c>
       <c r="E5" t="s">
-        <v>266</v>
+        <v>374</v>
       </c>
       <c r="F5" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>126</v>
@@ -4397,8 +4606,11 @@
       <c r="H5" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I5" s="8" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>234</v>
       </c>
@@ -4412,19 +4624,22 @@
         <v>-77.565303900000004</v>
       </c>
       <c r="E6" t="s">
-        <v>269</v>
+        <v>376</v>
       </c>
       <c r="F6" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="G6" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="H6" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+        <v>265</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>234</v>
       </c>
@@ -4438,10 +4653,10 @@
         <v>-77.547101999999995</v>
       </c>
       <c r="E7" t="s">
-        <v>258</v>
+        <v>370</v>
       </c>
       <c r="F7" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>126</v>
@@ -4449,8 +4664,11 @@
       <c r="H7" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>250</v>
       </c>
@@ -4464,19 +4682,22 @@
         <v>-77.158857999999995</v>
       </c>
       <c r="E8" t="s">
-        <v>274</v>
+        <v>378</v>
       </c>
       <c r="F8" t="s">
-        <v>275</v>
+        <v>381</v>
       </c>
       <c r="G8" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="H8" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>269</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>250</v>
       </c>
@@ -4490,19 +4711,22 @@
         <v>-77.471795599999993</v>
       </c>
       <c r="E9" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="F9" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="G9" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H9" t="s">
-        <v>277</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I8" r:id="rId1" xr:uid="{00A9F6FD-843D-E447-AB89-D3DB3D52A89D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
mental health free map
</commit_message>
<xml_diff>
--- a/shinyapp/data/resourcecost.xlsx
+++ b/shinyapp/data/resourcecost.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amandaljuba/Downloads/DSPG-R-Training/2022_DSPG_Loudoun/shinyapp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE72AAB6-E829-3648-80DE-00D7FAB5C254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{00210173-BB87-4346-9F92-35349E8E9700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="500" windowWidth="14340" windowHeight="16280" firstSheet="1" activeTab="3" xr2:uid="{BAAF709D-C9C5-8D48-B85E-C6C35467C9B5}"/>
+    <workbookView xWindow="820" yWindow="500" windowWidth="14340" windowHeight="16260" firstSheet="1" activeTab="5" xr2:uid="{BAAF709D-C9C5-8D48-B85E-C6C35467C9B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Health Free" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="384">
   <si>
     <t>Food Pantry</t>
   </si>
@@ -1190,6 +1190,9 @@
   </si>
   <si>
     <t>Address4</t>
+  </si>
+  <si>
+    <t>https://www.prisonfellowship.org/</t>
   </si>
 </sst>
 </file>
@@ -3762,7 +3765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE608C9-15CC-5E48-B239-366E0A11B3B1}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -4459,8 +4462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6631F4BE-4E4B-894D-9D61-34BE7B78F59B}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4721,6 +4724,9 @@
       </c>
       <c r="H9" s="3" t="s">
         <v>126</v>
+      </c>
+      <c r="I9" t="s">
+        <v>383</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed fam eng map and made changes to headings on resources
</commit_message>
<xml_diff>
--- a/shinyapp/data/resourcecost.xlsx
+++ b/shinyapp/data/resourcecost.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amandaljuba/Downloads/DSPG-R-Training/2022_DSPG_Loudoun/shinyapp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF48A52-47BE-174D-A9C7-4BE42128AE01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2628F36-CC64-4245-A962-7473B24864C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="500" windowWidth="14340" windowHeight="16260" firstSheet="2" activeTab="7" xr2:uid="{BAAF709D-C9C5-8D48-B85E-C6C35467C9B5}"/>
+    <workbookView xWindow="13520" yWindow="500" windowWidth="14340" windowHeight="16260" firstSheet="2" activeTab="7" xr2:uid="{BAAF709D-C9C5-8D48-B85E-C6C35467C9B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Health Free" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Family" sheetId="4" r:id="rId7"/>
     <sheet name="Family Free" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="516">
   <si>
     <t>Food Pantry</t>
   </si>
@@ -1195,9 +1195,6 @@
     <t>https://www.prisonfellowship.org/</t>
   </si>
   <si>
-    <t>Housing utilities</t>
-  </si>
-  <si>
     <t>1 Harrison Street Southeast, Leesburg, VA 20175</t>
   </si>
   <si>
@@ -1292,9 +1289,6 @@
   </si>
   <si>
     <t>All community</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family Education </t>
   </si>
   <si>
     <t>Loudoun Nurturing Parenting Program</t>
@@ -1438,9 +1432,6 @@
     <t>www.inmed.org</t>
   </si>
   <si>
-    <t>Eseentials supply</t>
-  </si>
-  <si>
     <t>INMED Free Family Essentials and COVID Relief</t>
   </si>
   <si>
@@ -1464,9 +1455,6 @@
   </si>
   <si>
     <t>http://library.loudoun.gov</t>
-  </si>
-  <si>
-    <t>Employment</t>
   </si>
   <si>
     <t>8 South Street, SW
@@ -1532,21 +1520,6 @@
     <t>127 Briarwood Court, Sterling, VA 20164</t>
   </si>
   <si>
-    <t>20684 Ashburn Road, Ashburn, VA 20147</t>
-  </si>
-  <si>
-    <t>703 - 724-1555</t>
-  </si>
-  <si>
-    <t>Family Transitional Housing</t>
-  </si>
-  <si>
-    <t>Family Transitional Home program by Good Shepherd of Northern Virginia  is set up to transition residents into permanent, affordable housing.This program provides:- Transitional housing, shelter for women and children</t>
-  </si>
-  <si>
-    <t>https://goodshepherdnova.org/our-programs/</t>
-  </si>
-  <si>
     <t>302 Parker Court SE, Leesburg, VA 20175</t>
   </si>
   <si>
@@ -1559,69 +1532,24 @@
     <t>www.mobile-hope.org</t>
   </si>
   <si>
-    <t>Childcare</t>
-  </si>
-  <si>
-    <t>Virtual and Interactive learning labs</t>
-  </si>
-  <si>
-    <t>Help pay for childcare</t>
-  </si>
-  <si>
-    <t> Program's Website</t>
-  </si>
-  <si>
-    <t>Mon - Fri 7 am - 6 pm</t>
-  </si>
-  <si>
-    <t>Women, Infants and Children (WIC)Women, Infants and Children (WIC)</t>
-  </si>
-  <si>
-    <t>Government Food benefits</t>
-  </si>
-  <si>
     <t>Program's Website</t>
   </si>
   <si>
-    <t>Mon - Fri 8 - 4 30</t>
-  </si>
-  <si>
-    <t>Food Benefit</t>
-  </si>
-  <si>
     <t>102 Heritage Way, N.E., Suite 200, Leesburg, VA 20176</t>
   </si>
   <si>
     <t xml:space="preserve"> Supplemental Nutrition Assistance Program (SNAP)Supplemental Nutrition Assistance Program (SNAP)</t>
   </si>
   <si>
-    <t>Medical Supplies</t>
-  </si>
-  <si>
     <t>Free Family Essentials and COVID ReliefFree Family Essentials and COVID Relief</t>
   </si>
   <si>
     <t xml:space="preserve">Mon - Fri 9 30 - 5 30 </t>
   </si>
   <si>
-    <t>Hearing Aid</t>
-  </si>
-  <si>
-    <t>2 Pidgeon Hill Drive, Sterling, VA 20165</t>
-  </si>
-  <si>
-    <t>The Gift of SOund</t>
-  </si>
-  <si>
-    <t>Books</t>
-  </si>
-  <si>
     <t>Mon - Fri 8 -5</t>
   </si>
   <si>
-    <t>SACS Thrift Stores (Share And Care Store)</t>
-  </si>
-  <si>
     <t>7611 Little River Turnpike, Annandale, VA 22003</t>
   </si>
   <si>
@@ -1659,13 +1587,22 @@
   </si>
   <si>
     <t>Serves8</t>
+  </si>
+  <si>
+    <t>Employment Help</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Education </t>
+  </si>
+  <si>
+    <t>Essentials Supply</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="29">
+  <fonts count="26">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1830,28 +1767,9 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF202124"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF351417"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Itc-avant-garde-gothic-pro"/>
-    </font>
-    <font>
-      <sz val="5"/>
-      <color theme="1"/>
-      <name val="Source Sans Pro"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1875,7 +1793,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1921,14 +1839,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1955,13 +1865,13 @@
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>34</xdr:row>
+          <xdr:row>31</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>35</xdr:row>
+          <xdr:row>32</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2005,13 +1915,13 @@
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>35</xdr:row>
+          <xdr:row>31</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>36</xdr:row>
+          <xdr:row>32</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -5490,58 +5400,58 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A708080-F10E-8B49-902F-0D4AF2F44406}">
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>527</v>
+        <v>503</v>
       </c>
       <c r="B1" t="s">
-        <v>528</v>
+        <v>504</v>
       </c>
       <c r="C1" t="s">
-        <v>532</v>
+        <v>508</v>
       </c>
       <c r="D1" t="s">
         <v>151</v>
       </c>
       <c r="E1" t="s">
-        <v>529</v>
+        <v>505</v>
       </c>
       <c r="F1" t="s">
-        <v>530</v>
+        <v>506</v>
       </c>
       <c r="G1" t="s">
-        <v>531</v>
+        <v>507</v>
       </c>
       <c r="H1" t="s">
-        <v>533</v>
+        <v>509</v>
       </c>
       <c r="I1" t="s">
-        <v>534</v>
+        <v>510</v>
       </c>
       <c r="J1" t="s">
         <v>159</v>
       </c>
       <c r="L1" t="s">
-        <v>535</v>
+        <v>511</v>
       </c>
       <c r="M1" t="s">
-        <v>536</v>
+        <v>512</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="16" customHeight="1">
       <c r="A2" t="s">
+        <v>401</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>384</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>385</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2">
@@ -5554,27 +5464,27 @@
         <v>-77.562010044107197</v>
       </c>
       <c r="G2" s="19" t="s">
+        <v>385</v>
+      </c>
+      <c r="H2" s="19" t="s">
         <v>386</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="I2" s="20" t="s">
         <v>387</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="L2" t="s">
         <v>388</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>389</v>
-      </c>
-      <c r="M2" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15">
       <c r="A3" t="s">
-        <v>384</v>
+        <v>401</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3">
@@ -5587,27 +5497,27 @@
         <v>-77.566373372942493</v>
       </c>
       <c r="G3" s="19" t="s">
+        <v>391</v>
+      </c>
+      <c r="H3" s="19" t="s">
         <v>392</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="I3" s="22" t="s">
         <v>393</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="L3" t="s">
         <v>394</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>395</v>
-      </c>
-      <c r="M3" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15">
       <c r="A4" t="s">
+        <v>396</v>
+      </c>
+      <c r="B4" t="s">
         <v>397</v>
-      </c>
-      <c r="B4" t="s">
-        <v>398</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4">
@@ -5620,16 +5530,16 @@
         <v>-77.540925888283695</v>
       </c>
       <c r="G4" s="19" t="s">
+        <v>398</v>
+      </c>
+      <c r="H4" s="19" t="s">
         <v>399</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="I4" s="22" t="s">
         <v>400</v>
       </c>
-      <c r="I4" s="22" t="s">
-        <v>401</v>
-      </c>
       <c r="L4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="M4" t="s">
         <v>166</v>
@@ -5637,10 +5547,10 @@
     </row>
     <row r="5" spans="1:13" ht="15">
       <c r="A5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -5652,16 +5562,16 @@
         <v>-77.540925888283695</v>
       </c>
       <c r="G5" s="19" t="s">
+        <v>402</v>
+      </c>
+      <c r="H5" s="19" t="s">
         <v>403</v>
       </c>
-      <c r="H5" s="19" t="s">
-        <v>404</v>
-      </c>
       <c r="I5" s="22" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="L5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="M5" t="s">
         <v>166</v>
@@ -5669,10 +5579,10 @@
     </row>
     <row r="6" spans="1:13" ht="15">
       <c r="A6" t="s">
-        <v>384</v>
+        <v>401</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6">
@@ -5685,30 +5595,30 @@
         <v>-77.736489240505904</v>
       </c>
       <c r="G6" s="19" t="s">
+        <v>405</v>
+      </c>
+      <c r="H6" s="19" t="s">
         <v>406</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="I6" s="19" t="s">
         <v>407</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="L6" s="19" t="s">
+        <v>394</v>
+      </c>
+      <c r="M6" s="19" t="s">
         <v>408</v>
-      </c>
-      <c r="L6" s="19" t="s">
-        <v>395</v>
-      </c>
-      <c r="M6" s="19" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15">
       <c r="A7" t="s">
+        <v>409</v>
+      </c>
+      <c r="B7" s="23" t="s">
         <v>410</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="C7" t="s">
         <v>411</v>
-      </c>
-      <c r="C7" t="s">
-        <v>412</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -5720,30 +5630,30 @@
         <v>-77.562813165687601</v>
       </c>
       <c r="G7" s="19" t="s">
+        <v>412</v>
+      </c>
+      <c r="H7" s="19" t="s">
         <v>413</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="I7" s="20" t="s">
         <v>414</v>
       </c>
-      <c r="I7" s="20" t="s">
+      <c r="L7" t="s">
+        <v>394</v>
+      </c>
+      <c r="M7" s="19" t="s">
         <v>415</v>
-      </c>
-      <c r="L7" t="s">
-        <v>395</v>
-      </c>
-      <c r="M7" s="19" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15">
       <c r="A8" t="s">
-        <v>417</v>
+        <v>514</v>
       </c>
       <c r="B8" s="23" t="s">
+        <v>410</v>
+      </c>
+      <c r="C8" t="s">
         <v>411</v>
-      </c>
-      <c r="C8" t="s">
-        <v>412</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -5755,30 +5665,30 @@
         <v>-77.562813165687601</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="L8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="M8" s="19" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15">
       <c r="A9" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B9" s="23" t="s">
+        <v>410</v>
+      </c>
+      <c r="C9" t="s">
         <v>411</v>
-      </c>
-      <c r="C9" t="s">
-        <v>412</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -5790,30 +5700,30 @@
         <v>-77.562813165687601</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="I9" s="20" t="s">
+        <v>414</v>
+      </c>
+      <c r="L9" t="s">
+        <v>394</v>
+      </c>
+      <c r="M9" s="19" t="s">
         <v>415</v>
-      </c>
-      <c r="L9" t="s">
-        <v>395</v>
-      </c>
-      <c r="M9" s="19" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15">
       <c r="A10" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B10" s="23" t="s">
+        <v>410</v>
+      </c>
+      <c r="C10" t="s">
         <v>411</v>
-      </c>
-      <c r="C10" t="s">
-        <v>412</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -5825,16 +5735,16 @@
         <v>-77.562813165687601</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="I10" s="20" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="L10" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="M10" s="19" t="s">
         <v>166</v>
@@ -5842,13 +5752,13 @@
     </row>
     <row r="11" spans="1:13" ht="15">
       <c r="A11" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B11" s="23" t="s">
+        <v>410</v>
+      </c>
+      <c r="C11" t="s">
         <v>411</v>
-      </c>
-      <c r="C11" t="s">
-        <v>412</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -5860,16 +5770,16 @@
         <v>-77.562813165687601</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="I11" s="20" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="L11" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="M11" s="19" t="s">
         <v>166</v>
@@ -5877,13 +5787,13 @@
     </row>
     <row r="12" spans="1:13" ht="15">
       <c r="A12" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B12" s="23" t="s">
+        <v>410</v>
+      </c>
+      <c r="C12" t="s">
         <v>411</v>
-      </c>
-      <c r="C12" t="s">
-        <v>412</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -5895,16 +5805,16 @@
         <v>-77.562813165687601</v>
       </c>
       <c r="G12" s="19" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="H12" s="19" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="I12" s="20" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="L12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="M12" s="19" t="s">
         <v>166</v>
@@ -5912,10 +5822,10 @@
     </row>
     <row r="13" spans="1:13" ht="15">
       <c r="A13" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C13" s="26"/>
       <c r="D13">
@@ -5928,21 +5838,21 @@
         <v>-77.569871180350702</v>
       </c>
       <c r="G13" s="19" t="s">
+        <v>429</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>430</v>
+      </c>
+      <c r="I13" s="20" t="s">
         <v>431</v>
-      </c>
-      <c r="H13" s="19" t="s">
-        <v>432</v>
-      </c>
-      <c r="I13" s="20" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="36" customHeight="1">
       <c r="A14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14">
@@ -5955,27 +5865,27 @@
         <v>-77.555034971164702</v>
       </c>
       <c r="G14" s="19" t="s">
+        <v>433</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>434</v>
+      </c>
+      <c r="I14" s="22" t="s">
         <v>435</v>
       </c>
-      <c r="H14" s="19" t="s">
+      <c r="L14" t="s">
         <v>436</v>
       </c>
-      <c r="I14" s="22" t="s">
+      <c r="M14" s="19" t="s">
         <v>437</v>
-      </c>
-      <c r="L14" t="s">
-        <v>438</v>
-      </c>
-      <c r="M14" s="19" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15">
       <c r="A15" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B15" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -5987,21 +5897,21 @@
         <v>-77.426874346022601</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="H15" s="19" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="I15" s="22" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15">
       <c r="A16" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B16" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -6013,21 +5923,21 @@
         <v>-77.487399999999994</v>
       </c>
       <c r="G16" s="19" t="s">
+        <v>442</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>443</v>
+      </c>
+      <c r="I16" s="22" t="s">
         <v>444</v>
-      </c>
-      <c r="H16" s="19" t="s">
-        <v>445</v>
-      </c>
-      <c r="I16" s="22" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="15">
       <c r="A17" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B17" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -6039,21 +5949,21 @@
         <v>-77.564637416464194</v>
       </c>
       <c r="G17" s="19" t="s">
+        <v>446</v>
+      </c>
+      <c r="H17" s="19" t="s">
+        <v>447</v>
+      </c>
+      <c r="I17" s="22" t="s">
         <v>448</v>
-      </c>
-      <c r="H17" s="19" t="s">
-        <v>449</v>
-      </c>
-      <c r="I17" s="22" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="15">
       <c r="A18" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B18" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -6065,30 +5975,30 @@
         <v>-77.469991169314895</v>
       </c>
       <c r="G18" s="19" t="s">
+        <v>449</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="I18" s="20" t="s">
         <v>451</v>
       </c>
-      <c r="H18" s="19" t="s">
-        <v>452</v>
-      </c>
-      <c r="I18" s="20" t="s">
-        <v>453</v>
-      </c>
       <c r="L18" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="M18" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="29" customHeight="1">
       <c r="A19" t="s">
-        <v>417</v>
+        <v>514</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C19" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -6100,16 +6010,16 @@
         <v>-77.401696999999999</v>
       </c>
       <c r="G19" s="28" t="s">
+        <v>454</v>
+      </c>
+      <c r="H19" s="28" t="s">
+        <v>455</v>
+      </c>
+      <c r="I19" s="8" t="s">
         <v>456</v>
       </c>
-      <c r="H19" s="28" t="s">
-        <v>457</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>458</v>
-      </c>
       <c r="L19" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="M19" t="s">
         <v>178</v>
@@ -6117,13 +6027,13 @@
     </row>
     <row r="20" spans="1:13" ht="32" customHeight="1">
       <c r="A20" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C20" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -6135,30 +6045,30 @@
         <v>-77.408413899999999</v>
       </c>
       <c r="G20" s="28" t="s">
+        <v>459</v>
+      </c>
+      <c r="H20" s="29" t="s">
+        <v>460</v>
+      </c>
+      <c r="I20" s="8" t="s">
         <v>461</v>
       </c>
-      <c r="H20" s="29" t="s">
-        <v>462</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>463</v>
-      </c>
       <c r="L20" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="M20" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="32" customHeight="1">
       <c r="A21" t="s">
-        <v>464</v>
+        <v>515</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C21" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -6170,30 +6080,30 @@
         <v>-77.408413899999999</v>
       </c>
       <c r="G21" s="28" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="H21" s="29" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="L21" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="M21" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="32" customHeight="1">
       <c r="A22" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C22" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -6205,27 +6115,27 @@
         <v>-77.408413899999999</v>
       </c>
       <c r="G22" s="28" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="H22" s="29" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="L22" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="M22" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="26" customHeight="1">
       <c r="A23" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="E23" s="28">
         <v>38.989677999999998</v>
@@ -6234,30 +6144,30 @@
         <v>-77.427879000000004</v>
       </c>
       <c r="G23" s="28" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="H23" s="28" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="L23" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="M23" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="183">
       <c r="A24" t="s">
-        <v>473</v>
+        <v>513</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="C24" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -6269,16 +6179,16 @@
         <v>-77.566093300000006</v>
       </c>
       <c r="G24" s="28" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="H24" s="29" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="L24" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="M24" t="s">
         <v>200</v>
@@ -6286,13 +6196,13 @@
     </row>
     <row r="25" spans="1:13" ht="102">
       <c r="A25" t="s">
-        <v>473</v>
+        <v>513</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -6304,21 +6214,21 @@
         <v>-77.541544200000004</v>
       </c>
       <c r="G25" s="28" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="H25" s="29" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15">
       <c r="A26" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="C26" s="30"/>
       <c r="D26">
@@ -6331,24 +6241,24 @@
         <v>-77.360856999999996</v>
       </c>
       <c r="G26" s="28" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="H26" s="28" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="96">
       <c r="A27" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -6360,24 +6270,24 @@
         <v>-77.394760070000004</v>
       </c>
       <c r="G27" s="28" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="H27" s="28" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="80">
       <c r="A28" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B28" s="31" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -6389,218 +6299,100 @@
         <v>-77.394760070000004</v>
       </c>
       <c r="G28" s="28" t="s">
+        <v>486</v>
+      </c>
+      <c r="H28" s="28" t="s">
+        <v>487</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="17">
+      <c r="A29" t="s">
+        <v>401</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>490</v>
       </c>
-      <c r="H28" s="28" t="s">
+      <c r="C29" s="32"/>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>39.110133927921197</v>
+      </c>
+      <c r="F29">
+        <v>-77.556985799931297</v>
+      </c>
+      <c r="G29" s="19" t="s">
         <v>491</v>
       </c>
-      <c r="I28" s="8" t="s">
+      <c r="H29" s="9" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" ht="15">
-      <c r="A29" t="s">
-        <v>420</v>
-      </c>
-      <c r="B29" s="32" t="s">
+      <c r="I29" s="8" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="15">
+      <c r="A30" t="s">
+        <v>421</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>495</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="G30" s="28" t="s">
+        <v>496</v>
+      </c>
+      <c r="I30" t="s">
         <v>494</v>
       </c>
-      <c r="C29" s="30" t="s">
-        <v>495</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="G29" s="28" t="s">
-        <v>496</v>
-      </c>
-      <c r="H29" s="33" t="s">
+      <c r="L30" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="15">
+      <c r="A31" t="s">
+        <v>421</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="G31" s="28" t="s">
         <v>497</v>
       </c>
-      <c r="I29" s="8" t="s">
+      <c r="I31" t="s">
+        <v>494</v>
+      </c>
+      <c r="L31" t="s">
         <v>498</v>
-      </c>
-      <c r="L29" t="s">
-        <v>395</v>
-      </c>
-      <c r="M29" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="17">
-      <c r="A30" t="s">
-        <v>402</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>499</v>
-      </c>
-      <c r="C30" s="34"/>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>39.110133927921197</v>
-      </c>
-      <c r="F30">
-        <v>-77.556985799931297</v>
-      </c>
-      <c r="G30" s="19" t="s">
-        <v>500</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>501</v>
-      </c>
-      <c r="I30" s="8" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="85">
-      <c r="A31" t="s">
-        <v>503</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="H31" s="28" t="s">
-        <v>505</v>
-      </c>
-      <c r="I31" s="8" t="s">
-        <v>506</v>
-      </c>
-      <c r="L31" t="s">
-        <v>507</v>
-      </c>
-      <c r="M31" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="15">
       <c r="A32" t="s">
-        <v>503</v>
+        <v>421</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>49</v>
+        <v>500</v>
       </c>
       <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="G32" s="28" t="s">
-        <v>508</v>
-      </c>
-      <c r="H32" s="28" t="s">
-        <v>509</v>
-      </c>
-      <c r="I32" t="s">
-        <v>510</v>
+        <v>0</v>
+      </c>
+      <c r="G32" t="s">
+        <v>501</v>
+      </c>
+      <c r="H32" t="s">
+        <v>502</v>
       </c>
       <c r="L32" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="15">
-      <c r="A33" t="s">
-        <v>512</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>513</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="G33" s="28" t="s">
-        <v>514</v>
-      </c>
-      <c r="I33" t="s">
-        <v>510</v>
-      </c>
-      <c r="L33" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="15">
-      <c r="A34" t="s">
-        <v>515</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="G34" s="28" t="s">
-        <v>516</v>
-      </c>
-      <c r="I34" t="s">
-        <v>510</v>
-      </c>
-      <c r="L34" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="15">
-      <c r="A35" t="s">
-        <v>518</v>
-      </c>
-      <c r="B35" t="s">
-        <v>519</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="G35" s="35" t="s">
-        <v>520</v>
-      </c>
-      <c r="L35" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="15">
-      <c r="A36" t="s">
-        <v>521</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="G36" s="35"/>
-      <c r="L36" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="68">
-      <c r="A37" t="s">
-        <v>521</v>
-      </c>
-      <c r="G37" s="36" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="15">
-      <c r="A38" t="s">
-        <v>521</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>524</v>
-      </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="G38" t="s">
-        <v>525</v>
-      </c>
-      <c r="H38" t="s">
-        <v>526</v>
-      </c>
-      <c r="L38" t="s">
-        <v>522</v>
+        <v>499</v>
       </c>
     </row>
   </sheetData>
@@ -6620,28 +6412,23 @@
     <hyperlink ref="I25" r:id="rId13" xr:uid="{F9FD68F8-F332-8D4F-BF6E-1F39654B968E}"/>
     <hyperlink ref="I26" r:id="rId14" display="http://www.thetincupfund.org/" xr:uid="{0DA7B991-0739-464F-ADDE-F2B0B9551685}"/>
     <hyperlink ref="I28" r:id="rId15" display="http://www.novadiaperbank.org/" xr:uid="{2C72A514-D090-B24A-95AB-CDB4A9338F00}"/>
-    <hyperlink ref="I29" r:id="rId16" xr:uid="{7A4314FC-3FCF-024D-B11F-9FB638921265}"/>
-    <hyperlink ref="I30" r:id="rId17" xr:uid="{F1E920FF-34EB-A74D-862C-221AE3336D61}"/>
-    <hyperlink ref="I4" r:id="rId18" xr:uid="{5547A062-1D1C-724A-AC30-1CE4D4C20C7B}"/>
-    <hyperlink ref="I8" r:id="rId19" xr:uid="{DE7255FF-E051-5040-A6BD-A77C4FC72CE9}"/>
-    <hyperlink ref="I7" r:id="rId20" xr:uid="{B9F79059-3B37-FD4E-A670-6957794A6696}"/>
-    <hyperlink ref="I12" r:id="rId21" xr:uid="{1465F34B-A998-1F42-BA59-C3091D86E125}"/>
-    <hyperlink ref="I11" r:id="rId22" xr:uid="{7EB19017-8F77-4A4E-BFDD-98C4ED3F7178}"/>
-    <hyperlink ref="I10" r:id="rId23" xr:uid="{D39EB76B-A85C-4F44-9F27-990E31AC8097}"/>
-    <hyperlink ref="I22" r:id="rId24" display="http://www.inmed.org/" xr:uid="{84588288-B49A-3243-9849-D6159DECFB06}"/>
-    <hyperlink ref="I20" r:id="rId25" display="http://www.inmed.org/" xr:uid="{9CA75B1A-1024-3C44-97B8-090298777ED6}"/>
-    <hyperlink ref="I21" r:id="rId26" display="http://www.inmed.org/" xr:uid="{8BD5CCB4-6109-BA41-9AA4-C2652693DEED}"/>
-    <hyperlink ref="I27" r:id="rId27" display="http://www.novadiaperbank.org/" xr:uid="{B4918A77-60FF-4948-A7B0-94EFD96243EB}"/>
-    <hyperlink ref="I31" r:id="rId28" location="1597350518575-7190bf4e-0db4" display="https://www.ymcadc.org/learninglabs/ - 1597350518575-7190bf4e-0db4" xr:uid="{E511A051-FD86-FA48-A67D-B115E5340FF6}"/>
-    <hyperlink ref="B32" r:id="rId29" display="https://www.google.com/maps/?q=45201+Research+Place,+Ashburn,+VA+20147/" xr:uid="{56E0F4C5-D876-0F4C-AE09-C2155A582A8B}"/>
-    <hyperlink ref="B33" r:id="rId30" display="https://www.google.com/maps/?q=102+Heritage+Way,+N.E.,+Suite+200,+Leesburg,+VA+20176/" xr:uid="{92D2BA20-A066-DD45-8ED0-D2DC28347446}"/>
-    <hyperlink ref="B34" r:id="rId31" display="https://www.google.com/maps/?q=21630+Ridgetop+Circle,+Sterling,+VA+20166/" xr:uid="{E3E5FA18-494C-DB4E-B6AA-2AA22DC9DF2B}"/>
-    <hyperlink ref="B36" r:id="rId32" display="https://www.google.com/maps/?q=21770+Beaumeade+Cir,+Ashburn,+VA+20147/" xr:uid="{68F39E2D-99FF-AE44-9703-37D334CC297E}"/>
-    <hyperlink ref="G37" r:id="rId33" display="https://www.findhelp.org/door-of-hope--sterling-va--sacs-thrift-stores-%2528share-and-care-store%2529/5746807600054272?postal=20163" xr:uid="{D2620B84-1E0B-C340-8336-C60105A0355D}"/>
-    <hyperlink ref="B38" r:id="rId34" display="https://www.google.com/maps/?q=7611+Little+River+Turnpike,+Annandale,+VA+22003/" xr:uid="{EDD8FF0F-1EE5-144E-A712-20ED5E4F9D90}"/>
+    <hyperlink ref="I29" r:id="rId16" xr:uid="{F1E920FF-34EB-A74D-862C-221AE3336D61}"/>
+    <hyperlink ref="I4" r:id="rId17" xr:uid="{5547A062-1D1C-724A-AC30-1CE4D4C20C7B}"/>
+    <hyperlink ref="I8" r:id="rId18" xr:uid="{DE7255FF-E051-5040-A6BD-A77C4FC72CE9}"/>
+    <hyperlink ref="I7" r:id="rId19" xr:uid="{B9F79059-3B37-FD4E-A670-6957794A6696}"/>
+    <hyperlink ref="I12" r:id="rId20" xr:uid="{1465F34B-A998-1F42-BA59-C3091D86E125}"/>
+    <hyperlink ref="I11" r:id="rId21" xr:uid="{7EB19017-8F77-4A4E-BFDD-98C4ED3F7178}"/>
+    <hyperlink ref="I10" r:id="rId22" xr:uid="{D39EB76B-A85C-4F44-9F27-990E31AC8097}"/>
+    <hyperlink ref="I22" r:id="rId23" display="http://www.inmed.org/" xr:uid="{84588288-B49A-3243-9849-D6159DECFB06}"/>
+    <hyperlink ref="I20" r:id="rId24" display="http://www.inmed.org/" xr:uid="{9CA75B1A-1024-3C44-97B8-090298777ED6}"/>
+    <hyperlink ref="I21" r:id="rId25" display="http://www.inmed.org/" xr:uid="{8BD5CCB4-6109-BA41-9AA4-C2652693DEED}"/>
+    <hyperlink ref="I27" r:id="rId26" display="http://www.novadiaperbank.org/" xr:uid="{B4918A77-60FF-4948-A7B0-94EFD96243EB}"/>
+    <hyperlink ref="B30" r:id="rId27" display="https://www.google.com/maps/?q=102+Heritage+Way,+N.E.,+Suite+200,+Leesburg,+VA+20176/" xr:uid="{92D2BA20-A066-DD45-8ED0-D2DC28347446}"/>
+    <hyperlink ref="B31" r:id="rId28" display="https://www.google.com/maps/?q=21630+Ridgetop+Circle,+Sterling,+VA+20166/" xr:uid="{E3E5FA18-494C-DB4E-B6AA-2AA22DC9DF2B}"/>
+    <hyperlink ref="B32" r:id="rId29" display="https://www.google.com/maps/?q=7611+Little+River+Turnpike,+Annandale,+VA+22003/" xr:uid="{EDD8FF0F-1EE5-144E-A712-20ED5E4F9D90}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId35"/>
-  <legacyDrawing r:id="rId36"/>
+  <drawing r:id="rId30"/>
+  <legacyDrawing r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>